<commit_message>
changed calculation of aggression
</commit_message>
<xml_diff>
--- a/TestGPoker/Config/Auswertungen-Tabea.xlsx
+++ b/TestGPoker/Config/Auswertungen-Tabea.xlsx
@@ -575,9 +575,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -586,19 +583,23 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>x</c:v>
+            <c:v>7c</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$9:$J$33</c:f>
+              <c:f>Tabelle1!$J$9:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.16933333333333334</c:v>
                 </c:pt>
@@ -616,73 +617,16 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.066666666666667E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.7666666666666668E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.12966666666666665</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.15033333333333335</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7.9000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.17233333333333334</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.12666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.109</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.21166666666666667</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.30633333333333335</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7.7666666666666676E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.64266666666666661</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.64866666666666661</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.6666666666666668E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8.9333333333333334E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.29599999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$L$9:$L$33</c:f>
+              <c:f>Tabelle1!$L$9:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.52033333333333331</c:v>
                 </c:pt>
@@ -700,73 +644,232 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.47766666666666668</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.55466666666666675</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.82233333333333336</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.34336666666666665</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.44500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.43933333333333335</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.51066666666666671</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.59233333333333338</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.45633333333333331</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.48533333333333334</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.66486666666666661</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.61099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.78866666666666674</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.28833333333333333</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.28799999999999998</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.97066666666666668</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.97766666666666657</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.88533333333333319</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.7897333333333334</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.52866666666666662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="109105536"/>
-        <c:axId val="109107456"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tester</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$J$15:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.066666666666667E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7666666666666668E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$L$15:$L$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.55466666666666675</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82233333333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34336666666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8a</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$J$18:$J$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.12966666666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15033333333333335</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17233333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$L$18:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.44500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43933333333333335</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51066666666666671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59233333333333338</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45633333333333331</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48533333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>9z</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$J$24:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.21166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30633333333333335</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7666666666666676E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64266666666666661</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64866666666666661</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6666666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29599999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$L$24:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.66486666666666661</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78866666666666674</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97066666666666668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97766666666666657</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88533333333333319</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7897333333333334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52866666666666662</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="103525760"/>
+        <c:axId val="110348160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109105536"/>
+        <c:axId val="103525760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -793,12 +896,12 @@
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109107456"/>
+        <c:crossAx val="110348160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109107456"/>
+        <c:axId val="110348160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -826,7 +929,7 @@
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109105536"/>
+        <c:crossAx val="103525760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -840,7 +943,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1168,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>